<commit_message>
adding heart age scoring table
</commit_message>
<xml_diff>
--- a/Cardiovascular Disease (10-year risk)2008.xlsx
+++ b/Cardiovascular Disease (10-year risk)2008.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14400" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14400" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Men" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="65">
   <si>
     <t>Table 7. CVD Points for Men</t>
   </si>
@@ -199,6 +199,30 @@
   </si>
   <si>
     <t xml:space="preserve">Circulation. 2008;117:743-753, originally published February 11, 2008 </t>
+  </si>
+  <si>
+    <t>Table 9. Heart Age/Vascular Age for Women</t>
+  </si>
+  <si>
+    <t>Heart Age, y</t>
+  </si>
+  <si>
+    <t>&lt;30</t>
+  </si>
+  <si>
+    <t>15+</t>
+  </si>
+  <si>
+    <t>&gt;80</t>
+  </si>
+  <si>
+    <t>Table 10. Heart Age/Vascular Age for Men</t>
+  </si>
+  <si>
+    <t>&lt;0</t>
+  </si>
+  <si>
+    <t>≥17</t>
   </si>
 </sst>
 </file>
@@ -467,7 +491,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -482,14 +506,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -503,29 +538,30 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -803,46 +839,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L29"/>
+  <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="12" max="12" width="12.1640625" customWidth="1"/>
+    <col min="14" max="14" width="17.6640625" customWidth="1"/>
+    <col min="15" max="15" width="19.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="15"/>
-      <c r="K1" s="10" t="s">
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="24"/>
+      <c r="K1" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="L1" s="11"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="16"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="17"/>
+      <c r="L1" s="21"/>
+      <c r="N1" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="O1" s="33"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" s="25"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="27"/>
       <c r="K2" s="4"/>
       <c r="L2" s="5"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N2" s="13"/>
+      <c r="O2" s="14"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -874,8 +918,14 @@
       <c r="L3" s="7" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N3" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="O3" s="16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
@@ -896,8 +946,14 @@
       <c r="L4" s="5" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N4" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="O4" s="14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>12</v>
       </c>
@@ -916,8 +972,14 @@
       <c r="L5" s="5">
         <v>1.1000000000000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N5" s="13">
+        <v>0</v>
+      </c>
+      <c r="O5" s="14">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>0</v>
       </c>
@@ -948,8 +1010,14 @@
       <c r="L6" s="5">
         <v>1.4</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N6" s="13">
+        <v>1</v>
+      </c>
+      <c r="O6" s="14">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>1</v>
       </c>
@@ -972,8 +1040,14 @@
       <c r="L7" s="5">
         <v>1.6</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N7" s="13">
+        <v>2</v>
+      </c>
+      <c r="O7" s="14">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>2</v>
       </c>
@@ -1000,8 +1074,14 @@
       <c r="L8" s="5">
         <v>1.9</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N8" s="13">
+        <v>3</v>
+      </c>
+      <c r="O8" s="14">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>3</v>
       </c>
@@ -1026,8 +1106,14 @@
       <c r="L9" s="5">
         <v>2.2999999999999998</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N9" s="13">
+        <v>4</v>
+      </c>
+      <c r="O9" s="14">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>4</v>
       </c>
@@ -1050,8 +1136,14 @@
       <c r="L10" s="5">
         <v>2.8</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N10" s="13">
+        <v>5</v>
+      </c>
+      <c r="O10" s="14">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>5</v>
       </c>
@@ -1072,8 +1164,14 @@
       <c r="L11" s="5">
         <v>3.3</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N11" s="13">
+        <v>6</v>
+      </c>
+      <c r="O11" s="14">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>6</v>
       </c>
@@ -1092,8 +1190,14 @@
       <c r="L12" s="5">
         <v>3.9</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N12" s="13">
+        <v>7</v>
+      </c>
+      <c r="O12" s="14">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>7</v>
       </c>
@@ -1110,8 +1214,14 @@
       <c r="L13" s="5">
         <v>4.7</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N13" s="13">
+        <v>8</v>
+      </c>
+      <c r="O13" s="14">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <v>8</v>
       </c>
@@ -1130,8 +1240,14 @@
       <c r="L14" s="5">
         <v>5.6</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N14" s="13">
+        <v>9</v>
+      </c>
+      <c r="O14" s="14">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
         <v>9</v>
       </c>
@@ -1148,8 +1264,14 @@
       <c r="L15" s="5">
         <v>6.7</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N15" s="13">
+        <v>10</v>
+      </c>
+      <c r="O15" s="14">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <v>10</v>
       </c>
@@ -1168,8 +1290,14 @@
       <c r="L16" s="5">
         <v>7.9</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N16" s="13">
+        <v>11</v>
+      </c>
+      <c r="O16" s="14">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
         <v>11</v>
       </c>
@@ -1188,8 +1316,14 @@
       <c r="L17" s="5">
         <v>9.4</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N17" s="13">
+        <v>12</v>
+      </c>
+      <c r="O17" s="14">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
         <v>12</v>
       </c>
@@ -1208,8 +1342,14 @@
       <c r="L18" s="5">
         <v>11.2</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N18" s="13">
+        <v>13</v>
+      </c>
+      <c r="O18" s="14">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
         <v>13</v>
       </c>
@@ -1226,8 +1366,14 @@
       <c r="L19" s="5">
         <v>13.2</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N19" s="13">
+        <v>14</v>
+      </c>
+      <c r="O19" s="14">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
         <v>14</v>
       </c>
@@ -1246,8 +1392,14 @@
       <c r="L20" s="5">
         <v>15.6</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N20" s="13">
+        <v>15</v>
+      </c>
+      <c r="O20" s="14">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
         <v>15</v>
       </c>
@@ -1266,26 +1418,38 @@
       <c r="L21" s="5">
         <v>18.399999999999999</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="18" t="s">
+      <c r="N21" s="13">
+        <v>16</v>
+      </c>
+      <c r="O21" s="14">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B22" s="19"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="20"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="12"/>
       <c r="K22" s="4">
         <v>15</v>
       </c>
       <c r="L22" s="5">
         <v>21.6</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N22" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="O22" s="18" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="K23" s="4">
         <v>16</v>
       </c>
@@ -1293,7 +1457,7 @@
         <v>25.3</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="K24" s="4">
         <v>17</v>
       </c>
@@ -1301,7 +1465,7 @@
         <v>29.4</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="K25" s="8" t="s">
         <v>42</v>
       </c>
@@ -1309,66 +1473,67 @@
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A26" s="29" t="s">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A26" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="B26" s="29"/>
-      <c r="C26" s="29"/>
-      <c r="D26" s="29"/>
-      <c r="E26" s="29"/>
-      <c r="F26" s="29"/>
-      <c r="G26" s="29"/>
-      <c r="H26" s="29"/>
-      <c r="I26" s="29"/>
-      <c r="J26" s="29"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A27" s="29" t="s">
+      <c r="B26" s="19"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="19"/>
+      <c r="J26" s="19"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A27" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="B27" s="29"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="29"/>
-      <c r="E27" s="29"/>
-      <c r="F27" s="29"/>
-      <c r="G27" s="29"/>
-      <c r="H27" s="29"/>
-      <c r="I27" s="29"/>
-      <c r="J27" s="29"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A28" s="29" t="s">
+      <c r="B27" s="19"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="19"/>
+      <c r="J27" s="19"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A28" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="B28" s="29"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29"/>
-      <c r="G28" s="29"/>
-      <c r="H28" s="29"/>
-      <c r="I28" s="29"/>
-      <c r="J28" s="29"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A29" s="29" t="s">
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A29" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="B29" s="29"/>
-      <c r="C29" s="29"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="29"/>
-      <c r="F29" s="29"/>
-      <c r="G29" s="29"/>
-      <c r="H29" s="29"/>
-      <c r="I29" s="29"/>
-      <c r="J29" s="29"/>
+      <c r="B29" s="19"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="A1:H2"/>
+    <mergeCell ref="N1:O1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1376,10 +1541,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M33"/>
+  <dimension ref="A1:P33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1390,39 +1555,46 @@
     <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.1640625" customWidth="1"/>
     <col min="13" max="13" width="13.33203125" customWidth="1"/>
+    <col min="15" max="16" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A1" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="15"/>
-      <c r="L1" s="25" t="s">
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="24"/>
+      <c r="L1" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="M1" s="26"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="16"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="17"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="22"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M1" s="24"/>
+      <c r="O1" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="P1" s="24"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A2" s="25"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="27"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="29"/>
+      <c r="O2" s="28"/>
+      <c r="P2" s="29"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -1448,14 +1620,20 @@
         <v>8</v>
       </c>
       <c r="I3" s="7"/>
-      <c r="L3" s="23" t="s">
+      <c r="L3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="M3" s="24" t="s">
+      <c r="M3" s="16" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O3" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="P3" s="16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>47</v>
       </c>
@@ -1467,14 +1645,20 @@
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="5"/>
-      <c r="L4" s="21" t="s">
+      <c r="L4" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="M4" s="22" t="s">
+      <c r="M4" s="14" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O4" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="P4" s="14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>48</v>
       </c>
@@ -1488,14 +1672,20 @@
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="5"/>
-      <c r="L5" s="21" t="s">
+      <c r="L5" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="M5" s="22">
+      <c r="M5" s="14">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O5" s="13">
+        <v>1</v>
+      </c>
+      <c r="P5" s="14">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
@@ -1509,14 +1699,20 @@
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="5"/>
-      <c r="L6" s="21">
+      <c r="L6" s="13">
         <v>0</v>
       </c>
-      <c r="M6" s="22">
+      <c r="M6" s="14">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O6" s="13">
+        <v>2</v>
+      </c>
+      <c r="P6" s="14">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>12</v>
       </c>
@@ -1532,14 +1728,20 @@
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="5"/>
-      <c r="L7" s="21">
+      <c r="L7" s="13">
         <v>1</v>
       </c>
-      <c r="M7" s="22">
+      <c r="M7" s="14">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O7" s="13">
+        <v>3</v>
+      </c>
+      <c r="P7" s="14">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>0</v>
       </c>
@@ -1563,14 +1765,20 @@
         <v>18</v>
       </c>
       <c r="I8" s="5"/>
-      <c r="L8" s="21">
+      <c r="L8" s="13">
         <v>2</v>
       </c>
-      <c r="M8" s="22">
+      <c r="M8" s="14">
         <v>1.7</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O8" s="13">
+        <v>4</v>
+      </c>
+      <c r="P8" s="14">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>1</v>
       </c>
@@ -1588,14 +1796,20 @@
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="5"/>
-      <c r="L9" s="21">
+      <c r="L9" s="13">
         <v>3</v>
       </c>
-      <c r="M9" s="22">
+      <c r="M9" s="14">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O9" s="13">
+        <v>5</v>
+      </c>
+      <c r="P9" s="14">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>2</v>
       </c>
@@ -1615,14 +1829,20 @@
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="5"/>
-      <c r="L10" s="21">
+      <c r="L10" s="13">
         <v>4</v>
       </c>
-      <c r="M10" s="22">
+      <c r="M10" s="14">
         <v>2.4</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O10" s="13">
+        <v>6</v>
+      </c>
+      <c r="P10" s="14">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>3</v>
       </c>
@@ -1640,14 +1860,20 @@
       </c>
       <c r="H11" s="3"/>
       <c r="I11" s="5"/>
-      <c r="L11" s="21">
+      <c r="L11" s="13">
         <v>5</v>
       </c>
-      <c r="M11" s="22">
+      <c r="M11" s="14">
         <v>2.8</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O11" s="13">
+        <v>7</v>
+      </c>
+      <c r="P11" s="14">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>4</v>
       </c>
@@ -1667,14 +1893,20 @@
         <v>28</v>
       </c>
       <c r="I12" s="5"/>
-      <c r="L12" s="21">
+      <c r="L12" s="13">
         <v>6</v>
       </c>
-      <c r="M12" s="22">
+      <c r="M12" s="14">
         <v>3.3</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O12" s="13">
+        <v>8</v>
+      </c>
+      <c r="P12" s="14">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>5</v>
       </c>
@@ -1694,14 +1926,20 @@
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="5"/>
-      <c r="L13" s="21">
+      <c r="L13" s="13">
         <v>7</v>
       </c>
-      <c r="M13" s="22">
+      <c r="M13" s="14">
         <v>3.9</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O13" s="13">
+        <v>9</v>
+      </c>
+      <c r="P13" s="14">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <v>6</v>
       </c>
@@ -1715,14 +1953,20 @@
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="I14" s="5"/>
-      <c r="L14" s="21">
+      <c r="L14" s="13">
         <v>8</v>
       </c>
-      <c r="M14" s="22">
+      <c r="M14" s="14">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O14" s="13">
+        <v>10</v>
+      </c>
+      <c r="P14" s="14">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
         <v>7</v>
       </c>
@@ -1738,14 +1982,20 @@
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="5"/>
-      <c r="L15" s="21">
+      <c r="L15" s="13">
         <v>9</v>
       </c>
-      <c r="M15" s="22">
+      <c r="M15" s="14">
         <v>5.3</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O15" s="13">
+        <v>11</v>
+      </c>
+      <c r="P15" s="14">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <v>8</v>
       </c>
@@ -1759,14 +2009,20 @@
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
       <c r="I16" s="5"/>
-      <c r="L16" s="21">
+      <c r="L16" s="13">
         <v>10</v>
       </c>
-      <c r="M16" s="22">
+      <c r="M16" s="14">
         <v>6.3</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O16" s="13">
+        <v>12</v>
+      </c>
+      <c r="P16" s="14">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
         <v>9</v>
       </c>
@@ -1780,14 +2036,20 @@
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="I17" s="5"/>
-      <c r="L17" s="21">
+      <c r="L17" s="13">
         <v>11</v>
       </c>
-      <c r="M17" s="22">
+      <c r="M17" s="14">
         <v>7.3</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O17" s="13">
+        <v>13</v>
+      </c>
+      <c r="P17" s="14">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
         <v>10</v>
       </c>
@@ -1801,14 +2063,20 @@
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
       <c r="I18" s="5"/>
-      <c r="L18" s="21">
+      <c r="L18" s="13">
         <v>12</v>
       </c>
-      <c r="M18" s="22">
+      <c r="M18" s="14">
         <v>8.6</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O18" s="30">
+        <v>14</v>
+      </c>
+      <c r="P18" s="31">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>11</v>
       </c>
@@ -1822,14 +2090,20 @@
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="5"/>
-      <c r="L19" s="21">
+      <c r="L19" s="13">
         <v>13</v>
       </c>
-      <c r="M19" s="22">
+      <c r="M19" s="14">
         <v>10</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O19" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="P19" s="18" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
         <v>12</v>
       </c>
@@ -1843,146 +2117,147 @@
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
       <c r="I20" s="5"/>
-      <c r="L20" s="21">
+      <c r="L20" s="13">
         <v>14</v>
       </c>
-      <c r="M20" s="22">
+      <c r="M20" s="14">
         <v>11.7</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="18" t="s">
+    <row r="21" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="19"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="19"/>
-      <c r="I21" s="20" t="s">
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="L21" s="21">
+      <c r="L21" s="13">
         <v>15</v>
       </c>
-      <c r="M21" s="22">
+      <c r="M21" s="14">
         <v>13.7</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="L22" s="21">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="L22" s="13">
         <v>16</v>
       </c>
-      <c r="M22" s="22">
+      <c r="M22" s="14">
         <v>15.9</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="L23" s="21">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="L23" s="13">
         <v>17</v>
       </c>
-      <c r="M23" s="22">
+      <c r="M23" s="14">
         <v>18.5</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="L24" s="21">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="L24" s="13">
         <v>18</v>
       </c>
-      <c r="M24" s="22">
+      <c r="M24" s="14">
         <v>21.5</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="L25" s="21">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="L25" s="13">
         <v>19</v>
       </c>
-      <c r="M25" s="22">
+      <c r="M25" s="14">
         <v>24.8</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="L26" s="21">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="L26" s="13">
         <v>20</v>
       </c>
-      <c r="M26" s="22">
+      <c r="M26" s="14">
         <v>28.5</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="L27" s="27" t="s">
+    <row r="27" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L27" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="M27" s="28" t="s">
+      <c r="M27" s="18" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A28" s="29" t="s">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A28" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="B28" s="29"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29"/>
-      <c r="G28" s="29"/>
-      <c r="H28" s="29"/>
-      <c r="I28" s="29"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A29" s="29" t="s">
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A29" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="B29" s="29"/>
-      <c r="C29" s="29"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="29"/>
-      <c r="F29" s="29"/>
-      <c r="G29" s="29"/>
-      <c r="H29" s="29"/>
-      <c r="I29" s="29"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A30" s="29" t="s">
+      <c r="B29" s="19"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A30" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="B30" s="29"/>
-      <c r="C30" s="29"/>
-      <c r="D30" s="29"/>
-      <c r="E30" s="29"/>
-      <c r="F30" s="29"/>
-      <c r="G30" s="29"/>
-      <c r="H30" s="29"/>
-      <c r="I30" s="29"/>
-      <c r="J30" s="29"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A31" s="29" t="s">
+      <c r="B30" s="19"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="19"/>
+      <c r="H30" s="19"/>
+      <c r="I30" s="19"/>
+      <c r="J30" s="19"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A31" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="B31" s="29"/>
-      <c r="C31" s="29"/>
-      <c r="D31" s="29"/>
-      <c r="E31" s="29"/>
-      <c r="F31" s="29"/>
-      <c r="G31" s="29"/>
-      <c r="H31" s="29"/>
-      <c r="I31" s="29"/>
-      <c r="J31" s="29"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="J32" s="29"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="19"/>
+      <c r="I31" s="19"/>
+      <c r="J31" s="19"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="J32" s="19"/>
     </row>
     <row r="33" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J33" s="29"/>
+      <c r="J33" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A1:I2"/>
-    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="L1:M2"/>
+    <mergeCell ref="O1:P2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
adding limits messages to parameters
</commit_message>
<xml_diff>
--- a/Cardiovascular Disease (10-year risk)2008.xlsx
+++ b/Cardiovascular Disease (10-year risk)2008.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="70">
   <si>
     <t>Table 7. CVD Points for Men</t>
   </si>
@@ -223,6 +223,21 @@
   </si>
   <si>
     <t>≥17</t>
+  </si>
+  <si>
+    <t>limits:</t>
+  </si>
+  <si>
+    <t>HDL must be between 10 and 100</t>
+  </si>
+  <si>
+    <t>Age must be between 30 and 74</t>
+  </si>
+  <si>
+    <t>Systolic pressure must be between 90 and 200</t>
+  </si>
+  <si>
+    <t>Total cholesterol must be between 100 and 405</t>
   </si>
 </sst>
 </file>
@@ -253,15 +268,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="19">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -487,11 +508,95 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -520,6 +625,12 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -544,23 +655,32 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -842,45 +962,48 @@
   <dimension ref="A1:O29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="4" max="4" width="16.5" customWidth="1"/>
+    <col min="5" max="5" width="15.5" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.1640625" customWidth="1"/>
     <col min="14" max="14" width="17.6640625" customWidth="1"/>
     <col min="15" max="15" width="19.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="24"/>
-      <c r="K1" s="20" t="s">
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="26"/>
+      <c r="K1" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="L1" s="21"/>
-      <c r="N1" s="32" t="s">
+      <c r="L1" s="23"/>
+      <c r="N1" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="O1" s="33"/>
+      <c r="O1" s="31"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" s="25"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="27"/>
+      <c r="A2" s="27"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="29"/>
       <c r="K2" s="4"/>
       <c r="L2" s="5"/>
       <c r="N2" s="13"/>
@@ -1426,16 +1549,16 @@
       </c>
     </row>
     <row r="22" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="12"/>
+      <c r="B22" s="35"/>
+      <c r="C22" s="35"/>
+      <c r="D22" s="35"/>
+      <c r="E22" s="35"/>
+      <c r="F22" s="35"/>
+      <c r="G22" s="35"/>
+      <c r="H22" s="36"/>
       <c r="K22" s="4">
         <v>15</v>
       </c>
@@ -1449,7 +1572,27 @@
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23" s="39" t="s">
+        <v>66</v>
+      </c>
+      <c r="D23" s="39" t="s">
+        <v>69</v>
+      </c>
+      <c r="E23" s="39" t="s">
+        <v>68</v>
+      </c>
+      <c r="F23" s="39" t="s">
+        <v>68</v>
+      </c>
+      <c r="G23" s="39"/>
+      <c r="H23" s="40"/>
       <c r="K23" s="4">
         <v>16</v>
       </c>
@@ -1466,6 +1609,7 @@
       </c>
     </row>
     <row r="25" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D25" s="37"/>
       <c r="K25" s="8" t="s">
         <v>42</v>
       </c>
@@ -1559,40 +1703,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="24"/>
-      <c r="L1" s="22" t="s">
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="26"/>
+      <c r="L1" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="M1" s="24"/>
-      <c r="O1" s="22" t="s">
+      <c r="M1" s="26"/>
+      <c r="O1" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="P1" s="24"/>
+      <c r="P1" s="26"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A2" s="25"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="27"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="29"/>
-      <c r="O2" s="28"/>
-      <c r="P2" s="29"/>
+      <c r="A2" s="27"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="29"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="33"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="33"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
@@ -2069,10 +2213,10 @@
       <c r="M18" s="14">
         <v>8.6</v>
       </c>
-      <c r="O18" s="30">
+      <c r="O18" s="20">
         <v>14</v>
       </c>
-      <c r="P18" s="31">
+      <c r="P18" s="21">
         <v>79</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add maximum and minimum values
</commit_message>
<xml_diff>
--- a/Cardiovascular Disease (10-year risk)2008.xlsx
+++ b/Cardiovascular Disease (10-year risk)2008.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14340" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Men" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="72">
   <si>
     <t>Table 7. CVD Points for Men</t>
   </si>
@@ -238,13 +238,19 @@
   </si>
   <si>
     <t>Total cholesterol must be between 100 and 405</t>
+  </si>
+  <si>
+    <t>maximum points</t>
+  </si>
+  <si>
+    <t>minimum points</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -263,6 +269,14 @@
     <font>
       <sz val="12"/>
       <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -596,7 +610,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -630,6 +644,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -667,21 +696,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -959,14 +974,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O29"/>
+  <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="A23:H23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="14.1640625" customWidth="1"/>
     <col min="4" max="4" width="16.5" customWidth="1"/>
     <col min="5" max="5" width="15.5" customWidth="1"/>
     <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
@@ -976,34 +992,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="26"/>
-      <c r="K1" s="22" t="s">
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="33"/>
+      <c r="K1" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="L1" s="23"/>
-      <c r="N1" s="30" t="s">
+      <c r="L1" s="30"/>
+      <c r="N1" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="O1" s="31"/>
+      <c r="O1" s="38"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" s="27"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="29"/>
+      <c r="A2" s="34"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="36"/>
       <c r="K2" s="4"/>
       <c r="L2" s="5"/>
       <c r="N2" s="13"/>
@@ -1549,16 +1565,16 @@
       </c>
     </row>
     <row r="22" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="34" t="s">
+      <c r="A22" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="B22" s="35"/>
-      <c r="C22" s="35"/>
-      <c r="D22" s="35"/>
-      <c r="E22" s="35"/>
-      <c r="F22" s="35"/>
-      <c r="G22" s="35"/>
-      <c r="H22" s="36"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="23"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="24"/>
       <c r="K22" s="4">
         <v>15</v>
       </c>
@@ -1573,26 +1589,26 @@
       </c>
     </row>
     <row r="23" spans="1:15" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="38" t="s">
+      <c r="A23" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="B23" s="39" t="s">
+      <c r="B23" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="C23" s="39" t="s">
+      <c r="C23" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="D23" s="39" t="s">
+      <c r="D23" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="E23" s="39" t="s">
+      <c r="E23" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="F23" s="39" t="s">
+      <c r="F23" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="G23" s="39"/>
-      <c r="H23" s="40"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="28"/>
       <c r="K23" s="4">
         <v>16</v>
       </c>
@@ -1608,32 +1624,28 @@
         <v>29.4</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D25" s="37"/>
-      <c r="K25" s="8" t="s">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A25" s="41" t="s">
+        <v>70</v>
+      </c>
+      <c r="B25" s="41">
+        <v>36</v>
+      </c>
+      <c r="K25" s="22"/>
+      <c r="L25" s="24"/>
+    </row>
+    <row r="26" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D26" s="25"/>
+      <c r="K26" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="L25" s="9" t="s">
+      <c r="L26" s="9" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A26" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="B26" s="19"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="19"/>
-      <c r="I26" s="19"/>
-      <c r="J26" s="19"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" s="19" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="B27" s="19"/>
       <c r="C27" s="19"/>
@@ -1647,7 +1659,7 @@
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B28" s="19"/>
       <c r="C28" s="19"/>
@@ -1661,7 +1673,7 @@
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" s="19" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="B29" s="19"/>
       <c r="C29" s="19"/>
@@ -1672,6 +1684,20 @@
       <c r="H29" s="19"/>
       <c r="I29" s="19"/>
       <c r="J29" s="19"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A30" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B30" s="19"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="19"/>
+      <c r="H30" s="19"/>
+      <c r="I30" s="19"/>
+      <c r="J30" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1687,8 +1713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1705,40 +1731,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="26"/>
-      <c r="L1" s="24" t="s">
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="33"/>
+      <c r="L1" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="M1" s="26"/>
-      <c r="O1" s="24" t="s">
+      <c r="M1" s="33"/>
+      <c r="O1" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="P1" s="26"/>
+      <c r="P1" s="33"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A2" s="27"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="29"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="33"/>
-      <c r="O2" s="32"/>
-      <c r="P2" s="33"/>
+      <c r="A2" s="34"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="36"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="40"/>
+      <c r="O2" s="39"/>
+      <c r="P2" s="40"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
@@ -2292,27 +2318,27 @@
       </c>
     </row>
     <row r="22" spans="1:16" ht="68" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="38" t="s">
+      <c r="A22" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="B22" s="39" t="s">
+      <c r="B22" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="C22" s="39" t="s">
+      <c r="C22" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="D22" s="39" t="s">
+      <c r="D22" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="E22" s="39" t="s">
+      <c r="E22" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="F22" s="39" t="s">
+      <c r="F22" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="G22" s="39"/>
-      <c r="H22" s="40"/>
-      <c r="I22" s="40"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="28"/>
+      <c r="I22" s="28"/>
       <c r="L22" s="13">
         <v>16</v>
       </c>
@@ -2329,6 +2355,12 @@
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A24" s="41" t="s">
+        <v>70</v>
+      </c>
+      <c r="B24" s="41">
+        <v>38</v>
+      </c>
       <c r="L24" s="13">
         <v>18</v>
       </c>
@@ -2337,6 +2369,12 @@
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A25" s="41" t="s">
+        <v>71</v>
+      </c>
+      <c r="B25" s="41">
+        <v>-6</v>
+      </c>
       <c r="L25" s="13">
         <v>19</v>
       </c>

</xml_diff>